<commit_message>
=countify addin - support for schedules
</commit_message>
<xml_diff>
--- a/Clients/CountifyExcel/GBP_Market.xlsx
+++ b/Clients/CountifyExcel/GBP_Market.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing_IRS" sheetId="7" r:id="rId1"/>
@@ -1597,7 +1597,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1725,9 +1725,7 @@
       <c r="A5" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="90" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="B5" s="123"/>
       <c r="C5" s="90" t="e">
         <v>#N/A</v>
       </c>
@@ -1759,9 +1757,7 @@
       <c r="A6" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="90" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="B6" s="123"/>
       <c r="C6" s="90" t="e">
         <v>#N/A</v>
       </c>
@@ -1970,13 +1966,13 @@
       <c r="A14" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="124" t="e">
-        <f ca="1">_xll.qlSchedule(,B4,B8,B9,B3,B10,B11,B12,B13,B5,B6,,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C14" s="124" t="e">
-        <f ca="1">_xll.qlSchedule(,C4,C8,C9,C3,C10,C11,C12,C13,C5,C6,,Trigger)</f>
-        <v>#NAME?</v>
+      <c r="B14" s="124" t="str">
+        <f>_xll.cfyql_Schedule("schedule1",B4,B8,B9,B3,B10,B11,B12,B13,B5,B6,,Trigger)</f>
+        <v>schedule1</v>
+      </c>
+      <c r="C14" s="124" t="str">
+        <f>_xll.cfyql_Schedule("schedule2",C4,C8,C9,C3,C10,C11,C12,C13,C5,C6,,Trigger)</f>
+        <v>schedule2</v>
       </c>
       <c r="D14" s="72"/>
       <c r="E14" s="72"/>
@@ -6127,7 +6123,7 @@
   </sheetPr>
   <dimension ref="A1:AB102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
fix some inputs in workbook
</commit_message>
<xml_diff>
--- a/Clients/CountifyExcel/GBP_Market.xlsx
+++ b/Clients/CountifyExcel/GBP_Market.xlsx
@@ -1637,10 +1637,10 @@
         <v>57</v>
       </c>
       <c r="B5" s="122">
-        <v>42180</v>
+        <v>42283</v>
       </c>
       <c r="C5" s="122">
-        <v>42180</v>
+        <v>42283</v>
       </c>
       <c r="D5" s="70" t="e">
         <f ca="1">SecondLegCF</f>
@@ -1669,8 +1669,12 @@
       <c r="A6" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="89" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
       <c r="C6" s="89" t="e">
+        <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D6" s="105" t="e">
@@ -1690,8 +1694,12 @@
       <c r="A7" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="89" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
       <c r="C7" s="89" t="e">
+        <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D7" s="71"/>
@@ -1725,10 +1733,10 @@
         <v>52</v>
       </c>
       <c r="B9" s="122">
-        <v>45833</v>
+        <v>45936</v>
       </c>
       <c r="C9" s="122">
-        <v>45833</v>
+        <v>45936</v>
       </c>
       <c r="D9" s="71"/>
       <c r="E9" s="71"/>
@@ -1980,10 +1988,12 @@
       <c r="A23" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="95" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C23" s="86" t="e">
+      <c r="B23" s="89" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C23" s="89" t="e">
+        <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D23" s="71"/>
@@ -2089,11 +2099,11 @@
         <v>31</v>
       </c>
       <c r="B29" s="91" t="e">
-        <f ca="1">_xll.cfyql_IborLeg("iborleg1",B17,SecondLegAdmortization_IRS!C6:C25,B15,NULL_ARRAY,B21,B22,NULL_ARRAY,NULL_ARRAY,B25,NULL_ARRAY,NULL_ARRAY)</f>
+        <f ca="1">_xll.cfyql_IborLeg("iborleg1",B17,SecondLegAdmortization_IRS!C6:C25,B15,NULL_ARRAY,B21,B22,B23,B24,B25,B26,NULL_ARRAY)</f>
         <v>#NAME?</v>
       </c>
       <c r="C29" s="86" t="e">
-        <f ca="1">_xll.cfyql_IborLeg("iborleg2",C17,SecondLegAdmortization_IRS!C6:C25,C15,NULL_ARRAY,C21,C22,NULL_ARRAY,NULL_ARRAY,C25,NULL_ARRAY,NULL_ARRAY)</f>
+        <f ca="1">_xll.cfyql_IborLeg("iborleg2",C17,SecondLegAdmortization_IRS!C6:C25,C15,NULL_ARRAY,C21,C22,NULL_ARRAY,C24,C25,C26,NULL_ARRAY)</f>
         <v>#NAME?</v>
       </c>
       <c r="D29" s="71"/>
@@ -2185,7 +2195,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="122">
-        <v>42180</v>
+        <v>42283</v>
       </c>
       <c r="C35" s="78"/>
       <c r="D35" s="71"/>
@@ -2201,7 +2211,7 @@
         <v>25</v>
       </c>
       <c r="B36" s="122">
-        <v>42180</v>
+        <v>42283</v>
       </c>
       <c r="C36" s="78"/>
       <c r="D36" s="71"/>

</xml_diff>

<commit_message>
fix glithc in spreadsheet
</commit_message>
<xml_diff>
--- a/Clients/CountifyExcel/GBP_Market.xlsx
+++ b/Clients/CountifyExcel/GBP_Market.xlsx
@@ -312,7 +312,7 @@
     <numFmt numFmtId="173" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="174" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +388,10 @@
       <sz val="8"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="13">
@@ -738,7 +742,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -790,8 +794,9 @@
     </xf>
     <xf numFmtId="172" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="172" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -942,9 +947,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="3" fillId="10" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="3" fillId="10" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="11" fillId="11" borderId="15" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -1017,7 +1019,6 @@
     <xf numFmtId="4" fontId="3" fillId="10" borderId="7" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="10" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="10" borderId="18" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="10" borderId="20" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="10" borderId="19" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="13" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1054,6 +1055,11 @@
     <xf numFmtId="174" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="10" borderId="20" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="10" borderId="11" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="11" fillId="11" borderId="15" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,7 +1067,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="5"/>
     <cellStyle name="Comma 3" xfId="6"/>
@@ -1089,6 +1095,7 @@
     <cellStyle name="Normal 6 2" xfId="26"/>
     <cellStyle name="Normal 7" xfId="27"/>
     <cellStyle name="Normal 8" xfId="28"/>
+    <cellStyle name="Normal 9" xfId="49"/>
     <cellStyle name="Normal_Pricing" xfId="29"/>
     <cellStyle name="Normale_AZIONI" xfId="30"/>
     <cellStyle name="Note 2" xfId="4"/>
@@ -1543,10 +1550,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="79" t="e">
+      <c r="B1" s="78" t="e">
         <f ca="1">SUM(MainChecks!D11:E16)</f>
         <v>#NAME?</v>
       </c>
@@ -1560,67 +1567,67 @@
       <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
       <c r="I2" s="69"/>
       <c r="J2" s="69"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="111" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="112" t="s">
+      <c r="D3" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="127" t="s">
+      <c r="F3" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="128"/>
+      <c r="G3" s="129"/>
       <c r="H3" s="69"/>
       <c r="I3" s="69"/>
       <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="110" t="e">
+      <c r="D4" s="108" t="e">
         <f ca="1">FirstLegCF</f>
         <v>#NAME?</v>
       </c>
-      <c r="E4" s="109" t="b">
+      <c r="E4" s="107" t="b">
         <f>B28</f>
         <v>1</v>
       </c>
-      <c r="F4" s="108">
-        <v>42180</v>
-      </c>
-      <c r="G4" s="107">
+      <c r="F4" s="125">
+        <v>42283</v>
+      </c>
+      <c r="G4" s="106">
         <v>0</v>
       </c>
       <c r="H4" s="69" t="e">
@@ -1633,27 +1640,27 @@
       <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="122">
+      <c r="B5" s="120">
         <v>42283</v>
       </c>
-      <c r="C5" s="122">
+      <c r="C5" s="120">
         <v>42283</v>
       </c>
       <c r="D5" s="70" t="e">
         <f ca="1">SecondLegCF</f>
         <v>#NAME?</v>
       </c>
-      <c r="E5" s="106" t="b">
+      <c r="E5" s="105" t="b">
         <f>C28</f>
         <v>0</v>
       </c>
-      <c r="F5" s="94">
-        <v>45833</v>
-      </c>
-      <c r="G5" s="93">
+      <c r="F5" s="126">
+        <v>45956</v>
+      </c>
+      <c r="G5" s="92">
         <v>0</v>
       </c>
       <c r="H5" s="69" t="e">
@@ -1666,192 +1673,192 @@
       <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="89" t="e">
+      <c r="B6" s="88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C6" s="89" t="e">
+      <c r="C6" s="88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="D6" s="105" t="e">
+      <c r="D6" s="104" t="e">
         <f ca="1">AdditionalCF</f>
         <v>#NAME?</v>
       </c>
-      <c r="E6" s="105" t="b">
+      <c r="E6" s="104" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="94"/>
-      <c r="G6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="92"/>
       <c r="H6" s="69"/>
       <c r="I6" s="69"/>
       <c r="J6" s="69"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="89" t="e">
+      <c r="B7" s="88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C7" s="89" t="e">
+      <c r="C7" s="88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D7" s="71"/>
       <c r="E7" s="71"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="92"/>
       <c r="H7" s="69"/>
       <c r="I7" s="69"/>
       <c r="J7" s="69"/>
     </row>
     <row r="8" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="103" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="71"/>
       <c r="E8" s="71"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="92"/>
       <c r="H8" s="69"/>
       <c r="I8" s="69"/>
       <c r="J8" s="69"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="122">
+      <c r="B9" s="120">
         <v>45936</v>
       </c>
-      <c r="C9" s="122">
+      <c r="C9" s="120">
         <v>45936</v>
       </c>
       <c r="D9" s="71"/>
       <c r="E9" s="71"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="92"/>
       <c r="H9" s="69"/>
       <c r="I9" s="69"/>
       <c r="J9" s="69"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="89" t="s">
+      <c r="C10" s="88" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="71"/>
       <c r="E10" s="71"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="92"/>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
       <c r="J10" s="69"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="89" t="s">
+      <c r="C11" s="88" t="s">
         <v>65</v>
       </c>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="92"/>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
       <c r="J11" s="69"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C12" s="88" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="71"/>
       <c r="E12" s="71"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="92"/>
       <c r="H12" s="69"/>
       <c r="I12" s="69"/>
       <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="88" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="71"/>
       <c r="E13" s="71"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="92"/>
       <c r="H13" s="69"/>
       <c r="I13" s="69"/>
       <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="89" t="b">
+      <c r="B14" s="88" t="b">
         <v>0</v>
       </c>
-      <c r="C14" s="89" t="b">
+      <c r="C14" s="88" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="71"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="92"/>
       <c r="H14" s="69"/>
       <c r="I14" s="69"/>
       <c r="J14" s="69"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="123" t="e">
+      <c r="B15" s="121" t="e">
         <f ca="1">_xll.cfyql_Schedule("schedule1",B5,B9,B10,B4,B11,B12,B13,B14,B6,B7,,Trigger)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C15" s="123" t="e">
+      <c r="C15" s="121" t="e">
         <f ca="1">_xll.cfyql_Schedule("schedule2",C5,C9,C10,C4,C11,C12,C13,C14,C6,C7,,Trigger)</f>
         <v>#NAME?</v>
       </c>
       <c r="D15" s="71"/>
       <c r="E15" s="71"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="93"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="92"/>
       <c r="H15" s="69"/>
       <c r="I15" s="69"/>
       <c r="J15" s="69"/>
@@ -1862,11 +1869,11 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="73"/>
       <c r="B16" s="73"/>
-      <c r="C16" s="78"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="71"/>
       <c r="E16" s="71"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="92"/>
       <c r="H16" s="69"/>
       <c r="I16" s="69"/>
       <c r="J16" s="69"/>
@@ -1875,253 +1882,253 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="83" t="s">
+      <c r="C17" s="82" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="71"/>
       <c r="E17" s="71"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="93"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="92"/>
       <c r="H17" s="69"/>
       <c r="I17" s="69"/>
       <c r="J17" s="69"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="125"/>
+      <c r="M17" s="123"/>
+      <c r="N17" s="123"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="76" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="72">
         <v>1000000</v>
       </c>
-      <c r="C18" s="85">
+      <c r="C18" s="84">
         <v>1000000</v>
       </c>
       <c r="D18" s="71"/>
       <c r="E18" s="71"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="92"/>
       <c r="H18" s="69"/>
       <c r="I18" s="69"/>
       <c r="J18" s="69"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="102" t="s">
+      <c r="B19" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="80" t="s">
+      <c r="C19" s="79" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="71"/>
       <c r="E19" s="71"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="92"/>
       <c r="H19" s="69"/>
       <c r="I19" s="69"/>
       <c r="J19" s="69"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="101">
+      <c r="B20" s="100">
         <v>0</v>
       </c>
-      <c r="C20" s="100">
+      <c r="C20" s="99">
         <v>0</v>
       </c>
       <c r="D20" s="71"/>
       <c r="E20" s="71"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="92"/>
       <c r="H20" s="69"/>
       <c r="I20" s="69"/>
       <c r="J20" s="69"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="95" t="b">
+      <c r="B21" s="94" t="b">
         <v>0</v>
       </c>
-      <c r="C21" s="80" t="b">
+      <c r="C21" s="79" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="71"/>
       <c r="E21" s="71"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="92"/>
       <c r="H21" s="69"/>
       <c r="I21" s="69"/>
       <c r="J21" s="69"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="98" t="s">
+      <c r="C22" s="97" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="71"/>
       <c r="E22" s="71"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="92"/>
       <c r="H22" s="69"/>
       <c r="I22" s="69"/>
       <c r="J22" s="69"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="89" t="e">
+      <c r="B23" s="88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C23" s="89" t="e">
+      <c r="C23" s="88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D23" s="71"/>
       <c r="E23" s="71"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="92"/>
       <c r="H23" s="69"/>
       <c r="I23" s="69"/>
       <c r="J23" s="69"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="96">
+      <c r="B24" s="95">
         <v>0</v>
       </c>
-      <c r="C24" s="97">
+      <c r="C24" s="96">
         <v>1</v>
       </c>
       <c r="D24" s="71"/>
       <c r="E24" s="71"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="92"/>
       <c r="H24" s="69"/>
       <c r="I24" s="69"/>
       <c r="J24" s="69"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="96" t="s">
+      <c r="B25" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="80" t="s">
+      <c r="C25" s="79" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="71"/>
       <c r="E25" s="71"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="92"/>
       <c r="H25" s="69"/>
       <c r="I25" s="69"/>
       <c r="J25" s="69"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="95">
+      <c r="B26" s="94">
         <v>0</v>
       </c>
-      <c r="C26" s="86">
+      <c r="C26" s="85">
         <v>0</v>
       </c>
       <c r="D26" s="71"/>
       <c r="E26" s="71"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="92"/>
       <c r="H26" s="69"/>
       <c r="I26" s="69"/>
       <c r="J26" s="69"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="95" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C27" s="86" t="e">
+      <c r="B27" s="94" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C27" s="85" t="e">
         <v>#N/A</v>
       </c>
       <c r="D27" s="71"/>
       <c r="E27" s="71"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="92"/>
       <c r="H27" s="69"/>
       <c r="I27" s="69"/>
       <c r="J27" s="69"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="95" t="b">
+      <c r="B28" s="94" t="b">
         <v>1</v>
       </c>
-      <c r="C28" s="80" t="b">
+      <c r="C28" s="79" t="b">
         <v>0</v>
       </c>
       <c r="D28" s="71"/>
       <c r="E28" s="71"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="92"/>
       <c r="H28" s="69"/>
       <c r="I28" s="69"/>
       <c r="J28" s="69"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="92" t="s">
+      <c r="A29" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="91" t="e">
+      <c r="B29" s="90" t="e">
         <f ca="1">_xll.cfyql_IborLeg("iborleg1",B17,SecondLegAdmortization_IRS!C6:C25,B15,NULL_ARRAY,B21,B22,B23,B24,B25,B26,NULL_ARRAY)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C29" s="86" t="e">
+      <c r="C29" s="85" t="e">
         <f ca="1">_xll.cfyql_IborLeg("iborleg2",C17,SecondLegAdmortization_IRS!C6:C25,C15,NULL_ARRAY,C21,C22,NULL_ARRAY,C24,C25,C26,NULL_ARRAY)</f>
         <v>#NAME?</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="71"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="89" t="e">
+      <c r="F29" s="89"/>
+      <c r="G29" s="88" t="e">
         <f ca="1">_xll.cfyql_MultiPhaseLeg("multileg1",H4:H5,FALSE)</f>
         <v>#NAME?</v>
       </c>
-      <c r="H29" s="88"/>
+      <c r="H29" s="87"/>
       <c r="I29" s="69"/>
       <c r="J29" s="69"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="85" t="e">
+      <c r="B30" s="84" t="e">
         <f ca="1">_xll.cfyql_Swap("swap",$D$4:$D$6,$E$4:$E$6)</f>
         <v>#NAME?</v>
       </c>
@@ -2147,13 +2154,13 @@
       <c r="J31" s="69"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="85" t="s">
+      <c r="B32" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
       <c r="F32" s="69"/>
@@ -2163,9 +2170,9 @@
       <c r="J32" s="69"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="78"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="71"/>
       <c r="E33" s="71"/>
       <c r="F33" s="69"/>
@@ -2175,13 +2182,13 @@
       <c r="J33" s="69"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="84" t="s">
+      <c r="A34" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="85" t="b">
+      <c r="B34" s="84" t="b">
         <v>1</v>
       </c>
-      <c r="C34" s="78"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="71"/>
       <c r="E34" s="71"/>
       <c r="F34" s="69"/>
@@ -2191,13 +2198,13 @@
       <c r="J34" s="69"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="82" t="s">
+      <c r="A35" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="122">
+      <c r="B35" s="120">
         <v>42283</v>
       </c>
-      <c r="C35" s="78"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="69"/>
@@ -2207,13 +2214,13 @@
       <c r="J35" s="69"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="122">
+      <c r="B36" s="120">
         <v>42283</v>
       </c>
-      <c r="C36" s="78"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="71"/>
       <c r="E36" s="71"/>
       <c r="F36" s="69"/>
@@ -2223,14 +2230,14 @@
       <c r="J36" s="69"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="85" t="e">
+      <c r="B37" s="84" t="e">
         <f ca="1">_xll.cfyql_DiscountingSwapEngine("engine",DiscountCurve,IncludeSettlementDate,SettlementDate,NPVDate)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C37" s="78"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="71"/>
       <c r="E37" s="71"/>
       <c r="F37" s="69"/>
@@ -2240,14 +2247,14 @@
       <c r="J37" s="69"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="124" t="e">
+      <c r="B38" s="122" t="e">
         <f ca="1">_xll.cfyql_InstrumentSetPricingEngine(SwapID,B37)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C38" s="78"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="71"/>
       <c r="E38" s="71"/>
       <c r="F38" s="69"/>
@@ -2269,10 +2276,10 @@
       <c r="J39" s="69"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="76" t="e">
+      <c r="B40" s="127" t="e">
         <f ca="1">_xll.cfyql_InstrumentNPV(SwapID,B38)</f>
         <v>#NAME?</v>
       </c>
@@ -2338,7 +2345,7 @@
       <c r="D3" s="64">
         <v>1000000</v>
       </c>
-      <c r="E3" s="117"/>
+      <c r="E3" s="115"/>
       <c r="F3" s="63">
         <v>20</v>
       </c>
@@ -2362,7 +2369,7 @@
       <c r="D5" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="121" t="s">
+      <c r="E5" s="119" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="58" t="s">
@@ -2383,13 +2390,13 @@
       <c r="B6" s="51">
         <v>42180</v>
       </c>
-      <c r="C6" s="115">
+      <c r="C6" s="113">
         <v>1000000</v>
       </c>
       <c r="D6" s="55">
         <v>1000000</v>
       </c>
-      <c r="E6" s="120">
+      <c r="E6" s="118">
         <v>1000000</v>
       </c>
       <c r="F6" s="55">
@@ -2412,13 +2419,13 @@
       <c r="B7" s="51">
         <v>42367</v>
       </c>
-      <c r="C7" s="115">
+      <c r="C7" s="113">
         <v>1000000</v>
       </c>
       <c r="D7" s="50">
         <v>1000000</v>
       </c>
-      <c r="E7" s="119">
+      <c r="E7" s="117">
         <v>1000000</v>
       </c>
       <c r="F7" s="50">
@@ -2441,13 +2448,13 @@
       <c r="B8" s="51">
         <v>42548</v>
       </c>
-      <c r="C8" s="115">
+      <c r="C8" s="113">
         <v>1000000</v>
       </c>
       <c r="D8" s="50">
         <v>1000000</v>
       </c>
-      <c r="E8" s="119">
+      <c r="E8" s="117">
         <v>1000000</v>
       </c>
       <c r="F8" s="50">
@@ -2470,13 +2477,13 @@
       <c r="B9" s="51">
         <v>42732</v>
       </c>
-      <c r="C9" s="115">
+      <c r="C9" s="113">
         <v>1000000</v>
       </c>
       <c r="D9" s="50">
         <v>1000000</v>
       </c>
-      <c r="E9" s="119">
+      <c r="E9" s="117">
         <v>1000000</v>
       </c>
       <c r="F9" s="50">
@@ -2499,13 +2506,13 @@
       <c r="B10" s="51">
         <v>42912</v>
       </c>
-      <c r="C10" s="115">
+      <c r="C10" s="113">
         <v>1000000</v>
       </c>
       <c r="D10" s="50">
         <v>1000000</v>
       </c>
-      <c r="E10" s="119">
+      <c r="E10" s="117">
         <v>1000000</v>
       </c>
       <c r="F10" s="50">
@@ -2528,13 +2535,13 @@
       <c r="B11" s="51">
         <v>43096</v>
       </c>
-      <c r="C11" s="115">
+      <c r="C11" s="113">
         <v>1000000</v>
       </c>
       <c r="D11" s="50">
         <v>1000000</v>
       </c>
-      <c r="E11" s="119">
+      <c r="E11" s="117">
         <v>1000000</v>
       </c>
       <c r="F11" s="50">
@@ -2557,13 +2564,13 @@
       <c r="B12" s="51">
         <v>43276</v>
       </c>
-      <c r="C12" s="115">
+      <c r="C12" s="113">
         <v>1000000</v>
       </c>
       <c r="D12" s="50">
         <v>1000000</v>
       </c>
-      <c r="E12" s="119">
+      <c r="E12" s="117">
         <v>1000000</v>
       </c>
       <c r="F12" s="50">
@@ -2586,13 +2593,13 @@
       <c r="B13" s="51">
         <v>43461</v>
       </c>
-      <c r="C13" s="115">
+      <c r="C13" s="113">
         <v>1000000</v>
       </c>
       <c r="D13" s="50">
         <v>1000000</v>
       </c>
-      <c r="E13" s="119">
+      <c r="E13" s="117">
         <v>1000000</v>
       </c>
       <c r="F13" s="50">
@@ -2615,13 +2622,13 @@
       <c r="B14" s="51">
         <v>43641</v>
       </c>
-      <c r="C14" s="115">
+      <c r="C14" s="113">
         <v>1000000</v>
       </c>
       <c r="D14" s="50">
         <v>1000000</v>
       </c>
-      <c r="E14" s="119">
+      <c r="E14" s="117">
         <v>1000000</v>
       </c>
       <c r="F14" s="50">
@@ -2644,13 +2651,13 @@
       <c r="B15" s="51">
         <v>43826</v>
       </c>
-      <c r="C15" s="115">
+      <c r="C15" s="113">
         <v>1000000</v>
       </c>
       <c r="D15" s="50">
         <v>1000000</v>
       </c>
-      <c r="E15" s="119">
+      <c r="E15" s="117">
         <v>1000000</v>
       </c>
       <c r="F15" s="50">
@@ -2673,13 +2680,13 @@
       <c r="B16" s="51">
         <v>44007</v>
       </c>
-      <c r="C16" s="115">
+      <c r="C16" s="113">
         <v>1000000</v>
       </c>
       <c r="D16" s="50">
         <v>1000000</v>
       </c>
-      <c r="E16" s="119">
+      <c r="E16" s="117">
         <v>1000000</v>
       </c>
       <c r="F16" s="50">
@@ -2702,13 +2709,13 @@
       <c r="B17" s="51">
         <v>44194</v>
       </c>
-      <c r="C17" s="115">
+      <c r="C17" s="113">
         <v>1000000</v>
       </c>
       <c r="D17" s="50">
         <v>1000000</v>
       </c>
-      <c r="E17" s="119">
+      <c r="E17" s="117">
         <v>1000000</v>
       </c>
       <c r="F17" s="50">
@@ -2731,13 +2738,13 @@
       <c r="B18" s="51">
         <v>44372</v>
       </c>
-      <c r="C18" s="115">
+      <c r="C18" s="113">
         <v>1000000</v>
       </c>
       <c r="D18" s="50">
         <v>1000000</v>
       </c>
-      <c r="E18" s="119">
+      <c r="E18" s="117">
         <v>1000000</v>
       </c>
       <c r="F18" s="50">
@@ -2760,13 +2767,13 @@
       <c r="B19" s="51">
         <v>44559</v>
       </c>
-      <c r="C19" s="115">
+      <c r="C19" s="113">
         <v>1000000</v>
       </c>
       <c r="D19" s="50">
         <v>1000000</v>
       </c>
-      <c r="E19" s="119">
+      <c r="E19" s="117">
         <v>1000000</v>
       </c>
       <c r="F19" s="50">
@@ -2789,13 +2796,13 @@
       <c r="B20" s="51">
         <v>44739</v>
       </c>
-      <c r="C20" s="115">
+      <c r="C20" s="113">
         <v>1000000</v>
       </c>
       <c r="D20" s="50">
         <v>1000000</v>
       </c>
-      <c r="E20" s="119">
+      <c r="E20" s="117">
         <v>1000000</v>
       </c>
       <c r="F20" s="50">
@@ -2818,13 +2825,13 @@
       <c r="B21" s="51">
         <v>44923</v>
       </c>
-      <c r="C21" s="115">
+      <c r="C21" s="113">
         <v>1000000</v>
       </c>
       <c r="D21" s="50">
         <v>1000000</v>
       </c>
-      <c r="E21" s="119">
+      <c r="E21" s="117">
         <v>1000000</v>
       </c>
       <c r="F21" s="50">
@@ -2847,13 +2854,13 @@
       <c r="B22" s="51">
         <v>45103</v>
       </c>
-      <c r="C22" s="115">
+      <c r="C22" s="113">
         <v>1000000</v>
       </c>
       <c r="D22" s="50">
         <v>1000000</v>
       </c>
-      <c r="E22" s="119">
+      <c r="E22" s="117">
         <v>1000000</v>
       </c>
       <c r="F22" s="50">
@@ -2876,13 +2883,13 @@
       <c r="B23" s="51">
         <v>45287</v>
       </c>
-      <c r="C23" s="115">
+      <c r="C23" s="113">
         <v>1000000</v>
       </c>
       <c r="D23" s="50">
         <v>1000000</v>
       </c>
-      <c r="E23" s="119">
+      <c r="E23" s="117">
         <v>1000000</v>
       </c>
       <c r="F23" s="50">
@@ -2905,13 +2912,13 @@
       <c r="B24" s="51">
         <v>45468</v>
       </c>
-      <c r="C24" s="115">
+      <c r="C24" s="113">
         <v>1000000</v>
       </c>
       <c r="D24" s="50">
         <v>1000000</v>
       </c>
-      <c r="E24" s="119">
+      <c r="E24" s="117">
         <v>1000000</v>
       </c>
       <c r="F24" s="50">
@@ -2934,13 +2941,13 @@
       <c r="B25" s="51">
         <v>45653</v>
       </c>
-      <c r="C25" s="115">
+      <c r="C25" s="113">
         <v>1000000</v>
       </c>
       <c r="D25" s="50">
         <v>1000000</v>
       </c>
-      <c r="E25" s="119">
+      <c r="E25" s="117">
         <v>1000000</v>
       </c>
       <c r="F25" s="50">
@@ -2963,13 +2970,13 @@
       <c r="B26" s="51">
         <v>45833</v>
       </c>
-      <c r="C26" s="115" t="e">
+      <c r="C26" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D26" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E26" s="119" t="e">
+      <c r="E26" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F26" s="50" t="e">
@@ -2992,13 +2999,13 @@
       <c r="B27" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C27" s="115" t="e">
+      <c r="C27" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D27" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E27" s="119" t="e">
+      <c r="E27" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F27" s="50" t="e">
@@ -3021,13 +3028,13 @@
       <c r="B28" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C28" s="115" t="e">
+      <c r="C28" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D28" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E28" s="119" t="e">
+      <c r="E28" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F28" s="50" t="e">
@@ -3050,13 +3057,13 @@
       <c r="B29" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C29" s="115" t="e">
+      <c r="C29" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D29" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E29" s="119" t="e">
+      <c r="E29" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F29" s="50" t="e">
@@ -3079,13 +3086,13 @@
       <c r="B30" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C30" s="115" t="e">
+      <c r="C30" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D30" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E30" s="119" t="e">
+      <c r="E30" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F30" s="50" t="e">
@@ -3108,13 +3115,13 @@
       <c r="B31" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C31" s="115" t="e">
+      <c r="C31" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D31" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E31" s="119" t="e">
+      <c r="E31" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F31" s="50" t="e">
@@ -3137,13 +3144,13 @@
       <c r="B32" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C32" s="115" t="e">
+      <c r="C32" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D32" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E32" s="119" t="e">
+      <c r="E32" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F32" s="50" t="e">
@@ -3166,13 +3173,13 @@
       <c r="B33" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C33" s="115" t="e">
+      <c r="C33" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D33" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E33" s="119" t="e">
+      <c r="E33" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F33" s="50" t="e">
@@ -3195,13 +3202,13 @@
       <c r="B34" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C34" s="115" t="e">
+      <c r="C34" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D34" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E34" s="119" t="e">
+      <c r="E34" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F34" s="50" t="e">
@@ -3224,13 +3231,13 @@
       <c r="B35" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C35" s="115" t="e">
+      <c r="C35" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D35" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E35" s="119" t="e">
+      <c r="E35" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F35" s="50" t="e">
@@ -3253,13 +3260,13 @@
       <c r="B36" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C36" s="115" t="e">
+      <c r="C36" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D36" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E36" s="119" t="e">
+      <c r="E36" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F36" s="50" t="e">
@@ -3282,13 +3289,13 @@
       <c r="B37" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C37" s="115" t="e">
+      <c r="C37" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D37" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E37" s="119" t="e">
+      <c r="E37" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F37" s="50" t="e">
@@ -3311,13 +3318,13 @@
       <c r="B38" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C38" s="115" t="e">
+      <c r="C38" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D38" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E38" s="119" t="e">
+      <c r="E38" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F38" s="50" t="e">
@@ -3340,13 +3347,13 @@
       <c r="B39" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C39" s="115" t="e">
+      <c r="C39" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D39" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E39" s="119" t="e">
+      <c r="E39" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F39" s="50" t="e">
@@ -3369,13 +3376,13 @@
       <c r="B40" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C40" s="115" t="e">
+      <c r="C40" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D40" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E40" s="119" t="e">
+      <c r="E40" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F40" s="50" t="e">
@@ -3398,13 +3405,13 @@
       <c r="B41" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C41" s="115" t="e">
+      <c r="C41" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D41" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E41" s="119" t="e">
+      <c r="E41" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F41" s="50" t="e">
@@ -3427,13 +3434,13 @@
       <c r="B42" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C42" s="115" t="e">
+      <c r="C42" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D42" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E42" s="119" t="e">
+      <c r="E42" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F42" s="50" t="e">
@@ -3456,13 +3463,13 @@
       <c r="B43" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C43" s="115" t="e">
+      <c r="C43" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D43" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E43" s="119" t="e">
+      <c r="E43" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F43" s="50" t="e">
@@ -3485,13 +3492,13 @@
       <c r="B44" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C44" s="115" t="e">
+      <c r="C44" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D44" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E44" s="119" t="e">
+      <c r="E44" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F44" s="50" t="e">
@@ -3514,13 +3521,13 @@
       <c r="B45" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C45" s="115" t="e">
+      <c r="C45" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D45" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E45" s="119" t="e">
+      <c r="E45" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F45" s="50" t="e">
@@ -3543,13 +3550,13 @@
       <c r="B46" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C46" s="115" t="e">
+      <c r="C46" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D46" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E46" s="119" t="e">
+      <c r="E46" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F46" s="50" t="e">
@@ -3572,13 +3579,13 @@
       <c r="B47" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C47" s="115" t="e">
+      <c r="C47" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D47" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E47" s="119" t="e">
+      <c r="E47" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F47" s="50" t="e">
@@ -3601,13 +3608,13 @@
       <c r="B48" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C48" s="115" t="e">
+      <c r="C48" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D48" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E48" s="119" t="e">
+      <c r="E48" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F48" s="50" t="e">
@@ -3630,13 +3637,13 @@
       <c r="B49" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C49" s="115" t="e">
+      <c r="C49" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D49" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E49" s="119" t="e">
+      <c r="E49" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F49" s="50" t="e">
@@ -3659,13 +3666,13 @@
       <c r="B50" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C50" s="115" t="e">
+      <c r="C50" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D50" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E50" s="119" t="e">
+      <c r="E50" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F50" s="50" t="e">
@@ -3688,13 +3695,13 @@
       <c r="B51" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C51" s="115" t="e">
+      <c r="C51" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D51" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E51" s="119" t="e">
+      <c r="E51" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F51" s="50" t="e">
@@ -3717,13 +3724,13 @@
       <c r="B52" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C52" s="115" t="e">
+      <c r="C52" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D52" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E52" s="119" t="e">
+      <c r="E52" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F52" s="50" t="e">
@@ -3746,13 +3753,13 @@
       <c r="B53" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C53" s="115" t="e">
+      <c r="C53" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D53" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E53" s="119" t="e">
+      <c r="E53" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F53" s="50" t="e">
@@ -3775,13 +3782,13 @@
       <c r="B54" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C54" s="115" t="e">
+      <c r="C54" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D54" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E54" s="119" t="e">
+      <c r="E54" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F54" s="50" t="e">
@@ -3804,13 +3811,13 @@
       <c r="B55" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C55" s="115" t="e">
+      <c r="C55" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D55" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E55" s="119" t="e">
+      <c r="E55" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F55" s="50" t="e">
@@ -3833,13 +3840,13 @@
       <c r="B56" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C56" s="115" t="e">
+      <c r="C56" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D56" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E56" s="119" t="e">
+      <c r="E56" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F56" s="50" t="e">
@@ -3862,13 +3869,13 @@
       <c r="B57" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C57" s="115" t="e">
+      <c r="C57" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D57" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E57" s="119" t="e">
+      <c r="E57" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F57" s="50" t="e">
@@ -3891,13 +3898,13 @@
       <c r="B58" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C58" s="115" t="e">
+      <c r="C58" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D58" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E58" s="119" t="e">
+      <c r="E58" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F58" s="50" t="e">
@@ -3920,13 +3927,13 @@
       <c r="B59" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C59" s="115" t="e">
+      <c r="C59" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D59" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E59" s="119" t="e">
+      <c r="E59" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F59" s="50" t="e">
@@ -3949,13 +3956,13 @@
       <c r="B60" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C60" s="115" t="e">
+      <c r="C60" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D60" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E60" s="119" t="e">
+      <c r="E60" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F60" s="50" t="e">
@@ -3978,13 +3985,13 @@
       <c r="B61" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C61" s="115" t="e">
+      <c r="C61" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D61" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E61" s="119" t="e">
+      <c r="E61" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F61" s="50" t="e">
@@ -4007,13 +4014,13 @@
       <c r="B62" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C62" s="115" t="e">
+      <c r="C62" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D62" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E62" s="119" t="e">
+      <c r="E62" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F62" s="50" t="e">
@@ -4036,13 +4043,13 @@
       <c r="B63" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C63" s="115" t="e">
+      <c r="C63" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D63" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E63" s="119" t="e">
+      <c r="E63" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F63" s="50" t="e">
@@ -4065,13 +4072,13 @@
       <c r="B64" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C64" s="115" t="e">
+      <c r="C64" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D64" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E64" s="119" t="e">
+      <c r="E64" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F64" s="50" t="e">
@@ -4094,13 +4101,13 @@
       <c r="B65" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C65" s="115" t="e">
+      <c r="C65" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D65" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E65" s="119" t="e">
+      <c r="E65" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F65" s="50" t="e">
@@ -4123,13 +4130,13 @@
       <c r="B66" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C66" s="115" t="e">
+      <c r="C66" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D66" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E66" s="119" t="e">
+      <c r="E66" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F66" s="50" t="e">
@@ -4152,13 +4159,13 @@
       <c r="B67" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C67" s="115" t="e">
+      <c r="C67" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D67" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E67" s="119" t="e">
+      <c r="E67" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F67" s="50" t="e">
@@ -4181,13 +4188,13 @@
       <c r="B68" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C68" s="115" t="e">
+      <c r="C68" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D68" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E68" s="119" t="e">
+      <c r="E68" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F68" s="50" t="e">
@@ -4210,13 +4217,13 @@
       <c r="B69" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C69" s="115" t="e">
+      <c r="C69" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D69" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E69" s="119" t="e">
+      <c r="E69" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F69" s="50" t="e">
@@ -4239,13 +4246,13 @@
       <c r="B70" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C70" s="115" t="e">
+      <c r="C70" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D70" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E70" s="119" t="e">
+      <c r="E70" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F70" s="50" t="e">
@@ -4268,13 +4275,13 @@
       <c r="B71" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C71" s="115" t="e">
+      <c r="C71" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D71" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E71" s="119" t="e">
+      <c r="E71" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F71" s="50" t="e">
@@ -4297,13 +4304,13 @@
       <c r="B72" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C72" s="115" t="e">
+      <c r="C72" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D72" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E72" s="119" t="e">
+      <c r="E72" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F72" s="50" t="e">
@@ -4326,13 +4333,13 @@
       <c r="B73" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C73" s="115" t="e">
+      <c r="C73" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D73" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E73" s="119" t="e">
+      <c r="E73" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F73" s="50" t="e">
@@ -4355,13 +4362,13 @@
       <c r="B74" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C74" s="115" t="e">
+      <c r="C74" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D74" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E74" s="119" t="e">
+      <c r="E74" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F74" s="50" t="e">
@@ -4384,13 +4391,13 @@
       <c r="B75" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C75" s="115" t="e">
+      <c r="C75" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D75" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E75" s="119" t="e">
+      <c r="E75" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F75" s="50" t="e">
@@ -4413,13 +4420,13 @@
       <c r="B76" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C76" s="115" t="e">
+      <c r="C76" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D76" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E76" s="119" t="e">
+      <c r="E76" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F76" s="50" t="e">
@@ -4442,13 +4449,13 @@
       <c r="B77" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C77" s="115" t="e">
+      <c r="C77" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D77" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E77" s="119" t="e">
+      <c r="E77" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F77" s="50" t="e">
@@ -4471,13 +4478,13 @@
       <c r="B78" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C78" s="115" t="e">
+      <c r="C78" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D78" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E78" s="119" t="e">
+      <c r="E78" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F78" s="50" t="e">
@@ -4500,13 +4507,13 @@
       <c r="B79" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C79" s="115" t="e">
+      <c r="C79" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D79" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E79" s="119" t="e">
+      <c r="E79" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F79" s="50" t="e">
@@ -4529,13 +4536,13 @@
       <c r="B80" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C80" s="115" t="e">
+      <c r="C80" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D80" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E80" s="119" t="e">
+      <c r="E80" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F80" s="50" t="e">
@@ -4558,13 +4565,13 @@
       <c r="B81" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C81" s="115" t="e">
+      <c r="C81" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D81" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E81" s="119" t="e">
+      <c r="E81" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F81" s="50" t="e">
@@ -4587,13 +4594,13 @@
       <c r="B82" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C82" s="115" t="e">
+      <c r="C82" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D82" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E82" s="119" t="e">
+      <c r="E82" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F82" s="50" t="e">
@@ -4616,13 +4623,13 @@
       <c r="B83" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C83" s="115" t="e">
+      <c r="C83" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D83" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E83" s="119" t="e">
+      <c r="E83" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F83" s="50" t="e">
@@ -4645,13 +4652,13 @@
       <c r="B84" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C84" s="115" t="e">
+      <c r="C84" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D84" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E84" s="119" t="e">
+      <c r="E84" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F84" s="50" t="e">
@@ -4674,13 +4681,13 @@
       <c r="B85" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C85" s="115" t="e">
+      <c r="C85" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D85" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E85" s="119" t="e">
+      <c r="E85" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F85" s="50" t="e">
@@ -4703,13 +4710,13 @@
       <c r="B86" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C86" s="115" t="e">
+      <c r="C86" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D86" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E86" s="119" t="e">
+      <c r="E86" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F86" s="50" t="e">
@@ -4732,13 +4739,13 @@
       <c r="B87" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C87" s="115" t="e">
+      <c r="C87" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D87" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E87" s="119" t="e">
+      <c r="E87" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F87" s="50" t="e">
@@ -4761,13 +4768,13 @@
       <c r="B88" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C88" s="115" t="e">
+      <c r="C88" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D88" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E88" s="119" t="e">
+      <c r="E88" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F88" s="50" t="e">
@@ -4790,13 +4797,13 @@
       <c r="B89" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C89" s="115" t="e">
+      <c r="C89" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D89" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E89" s="119" t="e">
+      <c r="E89" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F89" s="50" t="e">
@@ -4819,13 +4826,13 @@
       <c r="B90" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C90" s="115" t="e">
+      <c r="C90" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D90" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E90" s="119" t="e">
+      <c r="E90" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F90" s="50" t="e">
@@ -4848,13 +4855,13 @@
       <c r="B91" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C91" s="115" t="e">
+      <c r="C91" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D91" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E91" s="119" t="e">
+      <c r="E91" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F91" s="50" t="e">
@@ -4877,13 +4884,13 @@
       <c r="B92" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C92" s="115" t="e">
+      <c r="C92" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D92" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E92" s="119" t="e">
+      <c r="E92" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F92" s="50" t="e">
@@ -4906,13 +4913,13 @@
       <c r="B93" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C93" s="115" t="e">
+      <c r="C93" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D93" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E93" s="119" t="e">
+      <c r="E93" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F93" s="50" t="e">
@@ -4935,13 +4942,13 @@
       <c r="B94" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C94" s="115" t="e">
+      <c r="C94" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D94" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E94" s="119" t="e">
+      <c r="E94" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F94" s="50" t="e">
@@ -4964,13 +4971,13 @@
       <c r="B95" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C95" s="115" t="e">
+      <c r="C95" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D95" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E95" s="119" t="e">
+      <c r="E95" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F95" s="50" t="e">
@@ -4993,13 +5000,13 @@
       <c r="B96" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C96" s="115" t="e">
+      <c r="C96" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D96" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E96" s="119" t="e">
+      <c r="E96" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F96" s="50" t="e">
@@ -5022,13 +5029,13 @@
       <c r="B97" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C97" s="115" t="e">
+      <c r="C97" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D97" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E97" s="119" t="e">
+      <c r="E97" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F97" s="50" t="e">
@@ -5051,13 +5058,13 @@
       <c r="B98" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C98" s="115" t="e">
+      <c r="C98" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D98" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E98" s="119" t="e">
+      <c r="E98" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F98" s="50" t="e">
@@ -5080,13 +5087,13 @@
       <c r="B99" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C99" s="115" t="e">
+      <c r="C99" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D99" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E99" s="119" t="e">
+      <c r="E99" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F99" s="50" t="e">
@@ -5109,13 +5116,13 @@
       <c r="B100" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C100" s="115" t="e">
+      <c r="C100" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D100" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E100" s="119" t="e">
+      <c r="E100" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F100" s="50" t="e">
@@ -5138,13 +5145,13 @@
       <c r="B101" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C101" s="115" t="e">
+      <c r="C101" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D101" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E101" s="119" t="e">
+      <c r="E101" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F101" s="50" t="e">
@@ -5167,13 +5174,13 @@
       <c r="B102" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C102" s="115" t="e">
+      <c r="C102" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D102" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E102" s="119" t="e">
+      <c r="E102" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F102" s="50" t="e">
@@ -5196,13 +5203,13 @@
       <c r="B103" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C103" s="115" t="e">
+      <c r="C103" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D103" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E103" s="119" t="e">
+      <c r="E103" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F103" s="50" t="e">
@@ -5225,13 +5232,13 @@
       <c r="B104" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C104" s="115" t="e">
+      <c r="C104" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D104" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E104" s="119" t="e">
+      <c r="E104" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F104" s="50" t="e">
@@ -5254,13 +5261,13 @@
       <c r="B105" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C105" s="115" t="e">
+      <c r="C105" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D105" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E105" s="119" t="e">
+      <c r="E105" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F105" s="50" t="e">
@@ -5283,13 +5290,13 @@
       <c r="B106" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C106" s="115" t="e">
+      <c r="C106" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D106" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E106" s="119" t="e">
+      <c r="E106" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F106" s="50" t="e">
@@ -5312,13 +5319,13 @@
       <c r="B107" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C107" s="115" t="e">
+      <c r="C107" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D107" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E107" s="119" t="e">
+      <c r="E107" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F107" s="50" t="e">
@@ -5341,13 +5348,13 @@
       <c r="B108" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C108" s="115" t="e">
+      <c r="C108" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D108" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E108" s="119" t="e">
+      <c r="E108" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F108" s="50" t="e">
@@ -5370,13 +5377,13 @@
       <c r="B109" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C109" s="115" t="e">
+      <c r="C109" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D109" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E109" s="119" t="e">
+      <c r="E109" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F109" s="50" t="e">
@@ -5399,13 +5406,13 @@
       <c r="B110" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C110" s="115" t="e">
+      <c r="C110" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D110" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E110" s="119" t="e">
+      <c r="E110" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F110" s="50" t="e">
@@ -5428,13 +5435,13 @@
       <c r="B111" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C111" s="115" t="e">
+      <c r="C111" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D111" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E111" s="119" t="e">
+      <c r="E111" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F111" s="50" t="e">
@@ -5457,13 +5464,13 @@
       <c r="B112" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C112" s="115" t="e">
+      <c r="C112" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D112" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E112" s="119" t="e">
+      <c r="E112" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F112" s="50" t="e">
@@ -5486,13 +5493,13 @@
       <c r="B113" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C113" s="115" t="e">
+      <c r="C113" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D113" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E113" s="119" t="e">
+      <c r="E113" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F113" s="50" t="e">
@@ -5515,13 +5522,13 @@
       <c r="B114" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C114" s="115" t="e">
+      <c r="C114" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D114" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E114" s="119" t="e">
+      <c r="E114" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F114" s="50" t="e">
@@ -5544,13 +5551,13 @@
       <c r="B115" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C115" s="115" t="e">
+      <c r="C115" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D115" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E115" s="119" t="e">
+      <c r="E115" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F115" s="50" t="e">
@@ -5573,13 +5580,13 @@
       <c r="B116" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C116" s="115" t="e">
+      <c r="C116" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D116" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E116" s="119" t="e">
+      <c r="E116" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F116" s="50" t="e">
@@ -5602,13 +5609,13 @@
       <c r="B117" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C117" s="115" t="e">
+      <c r="C117" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D117" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E117" s="119" t="e">
+      <c r="E117" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F117" s="50" t="e">
@@ -5631,13 +5638,13 @@
       <c r="B118" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C118" s="115" t="e">
+      <c r="C118" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D118" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E118" s="119" t="e">
+      <c r="E118" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F118" s="50" t="e">
@@ -5660,13 +5667,13 @@
       <c r="B119" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C119" s="115" t="e">
+      <c r="C119" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D119" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E119" s="119" t="e">
+      <c r="E119" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F119" s="50" t="e">
@@ -5689,13 +5696,13 @@
       <c r="B120" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C120" s="115" t="e">
+      <c r="C120" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D120" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E120" s="119" t="e">
+      <c r="E120" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F120" s="50" t="e">
@@ -5718,13 +5725,13 @@
       <c r="B121" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C121" s="115" t="e">
+      <c r="C121" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D121" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E121" s="119" t="e">
+      <c r="E121" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F121" s="50" t="e">
@@ -5747,13 +5754,13 @@
       <c r="B122" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C122" s="115" t="e">
+      <c r="C122" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D122" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E122" s="119" t="e">
+      <c r="E122" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F122" s="50" t="e">
@@ -5776,13 +5783,13 @@
       <c r="B123" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C123" s="115" t="e">
+      <c r="C123" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D123" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E123" s="119" t="e">
+      <c r="E123" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F123" s="50" t="e">
@@ -5805,13 +5812,13 @@
       <c r="B124" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C124" s="115" t="e">
+      <c r="C124" s="113" t="e">
         <v>#N/A</v>
       </c>
       <c r="D124" s="50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E124" s="119" t="e">
+      <c r="E124" s="117" t="e">
         <v>#N/A</v>
       </c>
       <c r="F124" s="50" t="e">
@@ -5834,13 +5841,13 @@
       <c r="B125" s="47" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C125" s="114" t="e">
+      <c r="C125" s="112" t="e">
         <v>#N/A</v>
       </c>
       <c r="D125" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E125" s="118" t="e">
+      <c r="E125" s="116" t="e">
         <v>#N/A</v>
       </c>
       <c r="F125" s="46" t="e">
@@ -6010,7 +6017,7 @@
       <c r="L4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="126" t="e">
+      <c r="M4" s="124" t="e">
         <f ca="1">_xll.cfyql_SettingsEvaluationDate()</f>
         <v>#NAME?</v>
       </c>
@@ -9040,7 +9047,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9060,12 +9067,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9085,7 +9092,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>